<commit_message>
BOM Update and Controls Update
I added all the parts to the BOM that were used when I transistioned from a Pi3 to a Pi4 Build.  Also I decided to change the IPAC config from keyboard to a gamepad, I configured Steamlink and it does not like keyboards.  The gamepad switch required no additional config in any of the other cores.
</commit_message>
<xml_diff>
--- a/Documentation/Purchased Parts BOM.xlsx
+++ b/Documentation/Purchased Parts BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office\Google Drive\Documents\Arcade\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Arcade-Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tools" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Parts and Materials'!$A$1:$E$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Parts and Materials'!$A$1:$E$62</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="169">
   <si>
     <t>80mm Fan Grill</t>
   </si>
@@ -348,9 +348,6 @@
     <t>Sugatsune Mounting Plate</t>
   </si>
   <si>
-    <t>Delete unused once complete</t>
-  </si>
-  <si>
     <t>3/8" x 2 1/2" Hex Bolt</t>
   </si>
   <si>
@@ -390,15 +387,9 @@
     <t>MEL5_849black</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>GameonGrafix</t>
   </si>
   <si>
-    <t>Acrylic/Tempered Glass Bezel</t>
-  </si>
-  <si>
     <t>Switch Mount</t>
   </si>
   <si>
@@ -498,19 +489,52 @@
     <t>Raspberry Pi 4 4Gb</t>
   </si>
   <si>
-    <t>Sandisk 128Gb Flash Drive</t>
-  </si>
-  <si>
     <t>Pi4 4Gb</t>
   </si>
   <si>
-    <t>SDCZ48-128G-U46</t>
-  </si>
-  <si>
     <t>CanaKit 3.5A Raspberry Pi 4 Power Supply (USB-C)</t>
   </si>
   <si>
     <t>B07TYQRXTK</t>
+  </si>
+  <si>
+    <t>One Day Glass</t>
+  </si>
+  <si>
+    <t>.25" Thick Smoke Gray Tempered Glass</t>
+  </si>
+  <si>
+    <t>Geekworm Raspberry Pi 4 X862 M.2 NGFF SATA SSD Storage Expansion Board</t>
+  </si>
+  <si>
+    <t>Wathai Blue 100x100x2mm 2mm Silicone Pad Thermal Conductivity 1.5 W/mk</t>
+  </si>
+  <si>
+    <t>Arctic Silver 5 AS5-3.5G Thermal Paste</t>
+  </si>
+  <si>
+    <t>GeeekPi Raspberry Pi 4 Fan, Raspberry Pi Low-Profile CPU Cooler</t>
+  </si>
+  <si>
+    <t>Noctua NF-A4x10 5V, Premium Quiet Fan, 3-Pin, 5V Version</t>
+  </si>
+  <si>
+    <t>NF-A4x10 5V</t>
+  </si>
+  <si>
+    <t>B07ZV1LLWK</t>
+  </si>
+  <si>
+    <t>AS5-3.5G</t>
+  </si>
+  <si>
+    <t>B088HCY4TH</t>
+  </si>
+  <si>
+    <t>mDesign Modern Plastic Adhesive Cabinet and Wall Mount Storage Organizer Bin</t>
+  </si>
+  <si>
+    <t>9315MDKEU</t>
   </si>
 </sst>
 </file>
@@ -554,7 +578,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,12 +588,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -646,13 +664,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -938,11 +949,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,30 +980,30 @@
         <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="15"/>
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>54</v>
@@ -1001,7 +1012,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1009,7 +1020,7 @@
         <v>50</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>55</v>
@@ -1018,7 +1029,7 @@
         <v>64</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,7 +1037,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>56</v>
@@ -1035,7 +1046,7 @@
         <v>64</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1052,7 +1063,7 @@
         <v>62</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1069,7 +1080,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1161,7 +1172,7 @@
         <v>63</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1169,10 +1180,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>67</v>
@@ -1238,7 +1249,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>33</v>
@@ -1285,7 +1296,7 @@
         <v>63</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,16 +1304,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>64</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1319,7 +1330,7 @@
         <v>64</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1336,7 +1347,7 @@
         <v>64</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1353,7 +1364,7 @@
         <v>64</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1370,7 +1381,7 @@
         <v>64</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1387,7 +1398,7 @@
         <v>64</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1404,7 +1415,7 @@
         <v>64</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,10 +1426,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E29" s="6"/>
     </row>
@@ -1427,13 +1438,13 @@
         <v>8</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -1442,13 +1453,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -1457,47 +1468,47 @@
         <v>8</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>1</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>118</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>1</v>
       </c>
@@ -1512,7 +1523,7 @@
       </c>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>1</v>
       </c>
@@ -1527,37 +1538,37 @@
       </c>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>1</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>143</v>
+      <c r="B37" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="C37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>1</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
-        <v>1</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="C38" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>2</v>
       </c>
@@ -1565,14 +1576,14 @@
         <v>7233</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>1</v>
       </c>
@@ -1580,14 +1591,14 @@
         <v>33560</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>1</v>
       </c>
@@ -1595,14 +1606,14 @@
         <v>33566</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>3</v>
       </c>
@@ -1616,10 +1627,10 @@
         <v>99</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>3</v>
       </c>
@@ -1633,10 +1644,10 @@
         <v>99</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>3</v>
       </c>
@@ -1650,10 +1661,10 @@
         <v>99</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>25</v>
       </c>
@@ -1667,13 +1678,10 @@
         <v>99</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>3</v>
       </c>
@@ -1687,10 +1695,10 @@
         <v>66</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>2</v>
       </c>
@@ -1704,10 +1712,10 @@
         <v>66</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>2</v>
       </c>
@@ -1715,13 +1723,13 @@
         <v>49</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,13 +1740,13 @@
         <v>3221386</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1749,13 +1757,13 @@
         <v>3221386</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,13 +1774,13 @@
         <v>2751150</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1783,13 +1791,13 @@
         <v>2751148</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1806,7 +1814,7 @@
         <v>66</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1823,7 +1831,7 @@
         <v>67</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1855,7 +1863,7 @@
         <v>67</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1872,7 +1880,7 @@
         <v>67</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1905,37 +1913,37 @@
       </c>
       <c r="E59" s="6"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="6"/>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>1</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
-      <c r="B62" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="C62" s="8"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="D62" s="8"/>
       <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="6">
-        <v>1</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="A63" s="6"/>
+      <c r="B63" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
       <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1943,70 +1951,70 @@
         <v>1</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>153</v>
+        <v>31</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>131</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E64" s="6"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>1</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E65" s="6"/>
+        <v>129</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>1</v>
       </c>
       <c r="B66" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>1</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C67" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
+      <c r="D67" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="6">
-        <v>1</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="A68" s="6"/>
+      <c r="B68" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
       <c r="E68" s="6"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2014,55 +2022,76 @@
         <v>1</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>154</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>131</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E69" s="6"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>1</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>157</v>
+        <v>36</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E70" s="6"/>
+        <v>129</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>1</v>
       </c>
       <c r="B71" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>1</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C71" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E71" s="6"/>
+      <c r="D72" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" s="6"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D73" s="8"/>
+      <c r="A73" s="6">
+        <v>1</v>
+      </c>
+      <c r="B73" s="7">
+        <v>8541602182</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="E73" s="6"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2070,13 +2099,13 @@
         <v>1</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="E74" s="6"/>
     </row>
@@ -2085,18 +2114,87 @@
         <v>1</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="E75" s="6"/>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>1</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>1</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>1</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>1</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E81" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E61"/>
+  <autoFilter ref="A1:E62"/>
   <sortState ref="A2:E67">
     <sortCondition ref="D2:D67"/>
     <sortCondition ref="C2:C67"/>

</xml_diff>

<commit_message>
New PCBs, Added R1 files to Archive and Updated Documentation
Created a Archive folder and placed all R1 filesin it
Updated all the file in the documentation folder including PCB PDFs, BOM, Overall Schetmatic
Add the LCD Mount for the AUX control 2x20 Sxreen in the CAD Files Directory

PCB Chages:
3.5MM AUX Jack - Added PCB name/rev/date to the silkscreen
AUX Control - Added a 4 pin molex header to enable LCD output
Neopixel Control - Changed the switch resistor values from 1K to 10K to recude the voltage under 3.3V so the Teensy would register a switch interaction
Neopixel Developer - Changed the switch resistor values from 1K to 10K to recude the voltage under 3.3V so the Teensy would register a switch interaction.  Changed the GND Pin on all button switches (ABCXYZ SL ST OPT 1/2/3) as the NO switches conect across the button vs vertically
Overall Schetmatic - Changes RPI callout to Pi4

Created all new gerbers to order new PCBs
</commit_message>
<xml_diff>
--- a/Documentation/Purchased Parts BOM.xlsx
+++ b/Documentation/Purchased Parts BOM.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="162">
   <si>
     <t>80mm Fan Grill</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Molex 2 Position Rectangular Housing Connector</t>
   </si>
   <si>
-    <t>Molex 11 Position Rectangular Housing Connector</t>
-  </si>
-  <si>
     <t>Molex 4 Position Rectangular Housing Connector</t>
   </si>
   <si>
@@ -123,12 +120,6 @@
     <t>Monoprice 4' HDMI Cable</t>
   </si>
   <si>
-    <t>2.5A 5V Power Supply for Raspberry Pi</t>
-  </si>
-  <si>
-    <t>SAW-0512500</t>
-  </si>
-  <si>
     <t xml:space="preserve"> USB 2.0 A MALE TO MINI B RIGHT ANGLE UP</t>
   </si>
   <si>
@@ -141,18 +132,6 @@
     <t>Powerblock</t>
   </si>
   <si>
-    <t>Sandisk 128Gb MicroSD Card</t>
-  </si>
-  <si>
-    <t>SDSQUAR-128G-GN6MA</t>
-  </si>
-  <si>
-    <t>Raspberry Pi 3 B+</t>
-  </si>
-  <si>
-    <t>Pi3 B+</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -468,21 +447,9 @@
     <t>Power Cord - NEMA 5-15P to IEC 60320 C13, 18AWG, 10A/1250W, 125V, 3-Prong, 2ft</t>
   </si>
   <si>
-    <t>Raspberry Pi Options</t>
-  </si>
-  <si>
-    <t>Pi 3 Parts:</t>
-  </si>
-  <si>
     <t>Custom Parts</t>
   </si>
   <si>
-    <t>Pi 4 Parts:</t>
-  </si>
-  <si>
-    <t>Powerblock (Pi3) MicroUSB Version</t>
-  </si>
-  <si>
     <t>Powerblock (Pi4) USB-C Version</t>
   </si>
   <si>
@@ -535,6 +502,18 @@
   </si>
   <si>
     <t>9315MDKEU</t>
+  </si>
+  <si>
+    <t>LCD Mount</t>
+  </si>
+  <si>
+    <t>Mount for Aux Control PCB Support LCD</t>
+  </si>
+  <si>
+    <t>Molex 8 Position Rectangular Housing Connector</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Parts</t>
   </si>
 </sst>
 </file>
@@ -628,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -666,9 +645,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,11 +932,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60:XFD60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,19 +951,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -988,13 +971,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E2" s="6"/>
     </row>
@@ -1003,16 +986,16 @@
         <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1020,16 +1003,16 @@
         <v>50</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,16 +1020,16 @@
         <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,13 +1040,13 @@
         <v>4356</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,10 +1060,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1094,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E8" s="6"/>
     </row>
@@ -1106,10 +1089,10 @@
         <v>8541607606</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -1121,10 +1104,10 @@
         <v>4330172261</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -1139,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -1148,13 +1131,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E12" s="6"/>
     </row>
@@ -1163,16 +1146,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1180,13 +1163,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -1195,13 +1178,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E15" s="6"/>
     </row>
@@ -1210,13 +1193,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E16" s="6"/>
     </row>
@@ -1231,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E17" s="6"/>
     </row>
@@ -1246,10 +1229,10 @@
         <v>10</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,7 +1246,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E19" s="6"/>
     </row>
@@ -1278,7 +1261,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E20" s="6"/>
     </row>
@@ -1287,16 +1270,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1304,16 +1287,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1321,21 +1304,21 @@
         <v>2</v>
       </c>
       <c r="B23" s="7">
-        <v>9508111</v>
+        <v>9508080</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B24" s="7">
         <v>9508021</v>
@@ -1344,61 +1327,61 @@
         <v>16</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B25" s="7">
         <v>9508031</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B26" s="7">
         <v>9508041</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B27" s="7">
         <v>8500106</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1406,16 +1389,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1426,10 +1409,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E29" s="6"/>
     </row>
@@ -1438,13 +1421,13 @@
         <v>8</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -1453,13 +1436,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E31" s="6"/>
     </row>
@@ -1468,13 +1451,13 @@
         <v>8</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E32" s="6"/>
     </row>
@@ -1483,13 +1466,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E33" s="6"/>
     </row>
@@ -1498,13 +1481,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E34" s="6"/>
     </row>
@@ -1516,10 +1499,10 @@
         <v>5597</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -1531,10 +1514,10 @@
         <v>3992</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E36" s="6"/>
     </row>
@@ -1543,13 +1526,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -1558,13 +1541,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -1576,10 +1559,10 @@
         <v>7233</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E39" s="6"/>
     </row>
@@ -1591,10 +1574,10 @@
         <v>33560</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E40" s="6"/>
     </row>
@@ -1606,10 +1589,10 @@
         <v>33566</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E41" s="6"/>
     </row>
@@ -1618,16 +1601,16 @@
         <v>3</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1635,16 +1618,16 @@
         <v>3</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1652,16 +1635,16 @@
         <v>3</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1669,16 +1652,16 @@
         <v>25</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1686,16 +1669,16 @@
         <v>3</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1703,16 +1686,16 @@
         <v>2</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,16 +1703,16 @@
         <v>2</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1740,13 +1723,13 @@
         <v>3221386</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1757,13 +1740,13 @@
         <v>3221386</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1774,13 +1757,13 @@
         <v>2751150</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,13 +1774,13 @@
         <v>2751148</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1805,16 +1788,16 @@
         <v>1</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1822,16 +1805,16 @@
         <v>1</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1839,13 +1822,13 @@
         <v>3</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E55" s="6"/>
     </row>
@@ -1854,16 +1837,16 @@
         <v>1</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1871,16 +1854,16 @@
         <v>80</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1888,13 +1871,13 @@
         <v>2</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E58" s="6"/>
     </row>
@@ -1903,13 +1886,13 @@
         <v>3</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C59" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="E59" s="6"/>
     </row>
@@ -1918,13 +1901,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E60" s="6"/>
     </row>
@@ -1932,18 +1915,24 @@
       <c r="A62" s="6"/>
       <c r="B62" s="7"/>
       <c r="C62" s="16" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
+      <c r="A63" s="6">
+        <v>1</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1951,45 +1940,45 @@
         <v>1</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E64" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>1</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>128</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E65" s="6"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>1</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E66" s="6"/>
     </row>
@@ -1997,24 +1986,30 @@
       <c r="A67" s="6">
         <v>1</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>38</v>
+      <c r="B67" s="7">
+        <v>8541602182</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="6">
+        <v>1</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
+      <c r="D68" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E68" s="6"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2022,13 +2017,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E69" s="6"/>
     </row>
@@ -2037,61 +2032,38 @@
         <v>1</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>151</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>128</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E70" s="6"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>1</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E71" s="6"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="6">
-        <v>1</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E72" s="6"/>
-    </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="6">
-        <v>1</v>
-      </c>
-      <c r="B73" s="7">
-        <v>8541602182</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="8"/>
       <c r="E73" s="6"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2099,13 +2071,13 @@
         <v>1</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>160</v>
+        <v>8</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="E74" s="6"/>
     </row>
@@ -2114,84 +2086,30 @@
         <v>1</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="E75" s="6"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="6">
-        <v>1</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>162</v>
+      <c r="A76" s="17">
+        <v>1</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E76" s="6"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="6">
-        <v>1</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E77" s="6"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D79" s="8"/>
-      <c r="E79" s="6"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="6">
-        <v>1</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="6"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="6">
-        <v>1</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E81" s="6"/>
+        <v>114</v>
+      </c>
+      <c r="E76" s="17"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E62"/>
@@ -2223,16 +2141,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,13 +2158,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,13 +2172,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,13 +2186,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,13 +2200,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,13 +2214,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,13 +2228,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,13 +2242,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,13 +2256,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,13 +2270,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,13 +2284,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>